<commit_message>
updated some .xlsx files, deleted test.html, added region lists at app.py
</commit_message>
<xml_diff>
--- a/SCBAA/2016/NIR.xlsx
+++ b/SCBAA/2016/NIR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mngx\thesis\SCBA\Done XLSX - 2016\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mngx\Desktop\FlaskTuts\application\SCBAA\2016\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3088E1DE-331A-421D-9202-82F7E967F518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B3A032-67A6-4080-9FF8-374AD9B4219C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8730" yWindow="540" windowWidth="14625" windowHeight="12540" tabRatio="862" firstSheet="6" activeTab="11" xr2:uid="{55A92D14-81C0-4506-9860-A1CA671BF8C6}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="14625" windowHeight="12540" tabRatio="862" firstSheet="6" activeTab="7" xr2:uid="{55A92D14-81C0-4506-9860-A1CA671BF8C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Bacolod" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Cadiz" sheetId="5" r:id="rId5"/>
     <sheet name="Canlaon" sheetId="6" r:id="rId6"/>
     <sheet name="Dumaguete" sheetId="7" r:id="rId7"/>
-    <sheet name="Escalente" sheetId="8" r:id="rId8"/>
+    <sheet name="Escalante" sheetId="8" r:id="rId8"/>
     <sheet name="Guihulngan" sheetId="9" r:id="rId9"/>
     <sheet name="Himamaylan" sheetId="10" r:id="rId10"/>
     <sheet name="Kabankalan" sheetId="11" r:id="rId11"/>
@@ -36,6 +36,13 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -4795,7 +4802,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FFAD5C9-F430-45B7-8873-551817063EC9}">
   <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
@@ -20014,8 +20021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F690BC-511E-4BAE-A04E-56F6301F30A5}">
   <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E109" activeCellId="29" sqref="E10 E15 E20 E23 E28 E32 E41 E45 E49 E53 E57 E61 E65 E69 E73 E74 E77 E80 E83 E86 E89 E94 E95 E97 E99 E101 E103 E105 E107 E109"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>